<commit_message>
misc fixes after code review
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Partner_invoice_detail_template-v2-upcountry.xlsx
+++ b/application/controllers/excel-templates/Partner_invoice_detail_template-v2-upcountry.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28109"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Upcountry" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>

</xml_diff>

<commit_message>
Added both SF and customer pincode in Partner Upcountry Invoice
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Partner_invoice_detail_template-v2-upcountry.xlsx
+++ b/application/controllers/excel-templates/Partner_invoice_detail_template-v2-upcountry.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="28560" windowHeight="16400" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="28560" windowHeight="16340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Upcountry" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>ANNEXURE - UPCOUNTRY CHARGES</t>
   </si>
@@ -86,9 +86,6 @@
     <t>City</t>
   </si>
   <si>
-    <t>Pincode</t>
-  </si>
-  <si>
     <t>Upcountry Distance</t>
   </si>
   <si>
@@ -120,6 +117,17 @@
   </si>
   <si>
     <t>{meta:total_upcountry_price}</t>
+  </si>
+  <si>
+    <t>Customer 
+Pincode</t>
+  </si>
+  <si>
+    <t>Service Centre 
+Pincode</t>
+  </si>
+  <si>
+    <t>{booking:upcountry_pincode}</t>
   </si>
 </sst>
 </file>
@@ -137,38 +145,45 @@
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -332,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -405,6 +420,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -701,20 +719,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:D13"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="9.83203125" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="9" max="9" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -723,20 +741,22 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" ht="31" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
       <c r="H2" s="27"/>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I2" s="28"/>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="2"/>
@@ -744,9 +764,10 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="H3" s="2"/>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="6" t="s">
         <v>1</v>
@@ -756,9 +777,10 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H4" s="2"/>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="7"/>
       <c r="B5" s="8" t="s">
         <v>2</v>
@@ -766,13 +788,14 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="2"/>
+      <c r="G5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H5" s="2"/>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="7"/>
       <c r="B6" s="8" t="s">
         <v>4</v>
@@ -780,13 +803,14 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="2"/>
+      <c r="G6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H6" s="2"/>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="7"/>
       <c r="B7" s="8" t="s">
         <v>6</v>
@@ -794,23 +818,25 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="2"/>
+      <c r="G7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H7" s="2"/>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
       <c r="C8" s="9"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F8" s="2"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
       <c r="C9" s="9"/>
@@ -818,9 +844,10 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H9" s="2"/>
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="10"/>
       <c r="B10" s="11" t="s">
         <v>8</v>
@@ -828,13 +855,14 @@
       <c r="C10" s="9"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="2"/>
+      <c r="G10" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H10" s="2"/>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="12"/>
       <c r="B11" s="13" t="s">
         <v>10</v>
@@ -842,39 +870,42 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="2"/>
+      <c r="G11" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H11" s="2"/>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="12"/>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="12" t="s">
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H12" s="2"/>
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="12"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="12" t="s">
+      <c r="B13" s="31"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H13" s="2"/>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="12"/>
       <c r="B14" s="13" t="s">
         <v>14</v>
@@ -883,20 +914,22 @@
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G14" s="14"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="14"/>
       <c r="B15" s="15"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G15" s="14"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="14"/>
       <c r="B16" s="21" t="s">
         <v>15</v>
@@ -910,41 +943,47 @@
       <c r="E16" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="22" t="s">
+      <c r="F16" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="23" t="s">
+      <c r="I16" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="24" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="7"/>
       <c r="B17" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="D17" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="E17" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="F17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="H17" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="I17" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="H17" s="16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
       <c r="C18" s="2"/>
@@ -952,25 +991,27 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="4"/>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H18" s="2"/>
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="17"/>
       <c r="B19" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
       <c r="E19" s="19"/>
       <c r="F19" s="19"/>
       <c r="G19" s="19"/>
-      <c r="H19" s="20" t="s">
-        <v>30</v>
+      <c r="H19" s="19"/>
+      <c r="I19" s="20" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B2:I2"/>
     <mergeCell ref="B12:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
change excel column name Upcountry District
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Partner_invoice_detail_template-v2-upcountry.xlsx
+++ b/application/controllers/excel-templates/Partner_invoice_detail_template-v2-upcountry.xlsx
@@ -70,9 +70,6 @@
     <t>City</t>
   </si>
   <si>
-    <t>Service Centre City</t>
-  </si>
-  <si>
     <t>Service Centre 
 Pincode</t>
   </si>
@@ -81,6 +78,9 @@
 Pincode</t>
   </si>
   <si>
+    <t>Upcountry District</t>
+  </si>
+  <si>
     <t>Upcountry Distance</t>
   </si>
   <si>
@@ -99,13 +99,13 @@
     <t>{booking:city}</t>
   </si>
   <si>
+    <t>{booking:upcountry_pincode}</t>
+  </si>
+  <si>
+    <t>{booking:booking_pincode}</t>
+  </si>
+  <si>
     <t>{booking:upcountry_city}</t>
-  </si>
-  <si>
-    <t>{booking:upcountry_pincode}</t>
-  </si>
-  <si>
-    <t>{booking:booking_pincode}</t>
   </si>
   <si>
     <t>{booking:upcountry_distance}</t>
@@ -335,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -378,6 +378,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="6" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="7" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -397,6 +400,9 @@
     <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="13" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf borderId="7" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
@@ -407,10 +413,10 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="15" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="15" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="16" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -456,7 +462,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="3.0"/>
-    <col customWidth="1" min="2" max="7" width="14.43"/>
+    <col customWidth="1" min="2" max="6" width="14.43"/>
     <col customWidth="1" min="9" max="9" width="10.0"/>
     <col customWidth="1" min="10" max="10" width="9.71"/>
   </cols>
@@ -522,10 +528,10 @@
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="10" t="s">
+      <c r="G5" s="10" t="s">
         <v>3</v>
       </c>
+      <c r="H5" s="10"/>
       <c r="I5" s="5"/>
       <c r="J5" s="7"/>
     </row>
@@ -538,10 +544,10 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="10" t="s">
+      <c r="G6" s="10" t="s">
         <v>5</v>
       </c>
+      <c r="H6" s="10"/>
       <c r="I6" s="5"/>
       <c r="J6" s="7"/>
     </row>
@@ -554,10 +560,10 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="10" t="s">
+      <c r="G7" s="10" t="s">
         <v>7</v>
       </c>
+      <c r="H7" s="10"/>
       <c r="I7" s="5"/>
       <c r="J7" s="7"/>
     </row>
@@ -568,7 +574,7 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+      <c r="G8" s="10"/>
       <c r="H8" s="10"/>
       <c r="I8" s="5"/>
       <c r="J8" s="7"/>
@@ -594,112 +600,112 @@
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="15" t="s">
+      <c r="G10" s="15" t="s">
         <v>9</v>
       </c>
+      <c r="H10" s="16"/>
       <c r="I10" s="5"/>
       <c r="J10" s="7"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="15"/>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="10" t="s">
+      <c r="G11" s="10" t="s">
         <v>11</v>
       </c>
+      <c r="H11" s="10"/>
       <c r="I11" s="5"/>
       <c r="J11" s="7"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="15"/>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="15" t="s">
+      <c r="C12" s="19"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="15" t="s">
         <v>13</v>
       </c>
+      <c r="H12" s="16"/>
       <c r="I12" s="5"/>
       <c r="J12" s="7"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="15"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="15" t="s">
+      <c r="B13" s="23"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="15" t="s">
         <v>9</v>
       </c>
+      <c r="H13" s="16"/>
       <c r="I13" s="5"/>
       <c r="J13" s="7"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="15"/>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="26"/>
       <c r="I14" s="5"/>
       <c r="J14" s="7"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="21"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
+      <c r="A15" s="22"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="26"/>
       <c r="I15" s="5"/>
       <c r="J15" s="7"/>
     </row>
     <row r="16" ht="30.0" customHeight="1">
-      <c r="A16" s="21"/>
-      <c r="B16" s="26" t="s">
+      <c r="A16" s="22"/>
+      <c r="B16" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="27" t="s">
+      <c r="D16" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="27" t="s">
+      <c r="E16" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="28" t="s">
+      <c r="F16" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="29" t="s">
+      <c r="G16" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="29" t="s">
+      <c r="I16" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="30" t="s">
+      <c r="J16" s="32" t="s">
         <v>23</v>
       </c>
     </row>
@@ -717,19 +723,19 @@
       <c r="E17" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F17" s="31" t="s">
+      <c r="F17" s="10" t="s">
         <v>28</v>
       </c>
       <c r="G17" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="H17" s="33" t="s">
         <v>30</v>
       </c>
       <c r="I17" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="J17" s="32" t="s">
+      <c r="J17" s="34" t="s">
         <v>32</v>
       </c>
     </row>
@@ -746,18 +752,18 @@
       <c r="J18" s="7"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="33"/>
-      <c r="B19" s="34" t="s">
+      <c r="A19" s="35"/>
+      <c r="B19" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="36" t="s">
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="38" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
remove upcountry district from excel sheet
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Partner_invoice_detail_template-v2-upcountry.xlsx
+++ b/application/controllers/excel-templates/Partner_invoice_detail_template-v2-upcountry.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>ANNEXURE - UPCOUNTRY CHARGES</t>
   </si>
@@ -78,9 +78,6 @@
 Pincode</t>
   </si>
   <si>
-    <t>Upcountry District</t>
-  </si>
-  <si>
     <t>Upcountry Distance</t>
   </si>
   <si>
@@ -103,9 +100,6 @@
   </si>
   <si>
     <t>{booking:booking_pincode}</t>
-  </si>
-  <si>
-    <t>{booking:upcountry_city}</t>
   </si>
   <si>
     <t>{booking:upcountry_distance}</t>
@@ -335,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="35">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -380,9 +374,6 @@
     <xf borderId="6" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf borderId="7" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
@@ -400,9 +391,6 @@
     <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="13" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf borderId="7" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
@@ -415,14 +403,8 @@
     <xf borderId="15" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="15" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
     <xf borderId="16" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
@@ -463,8 +445,8 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="3.0"/>
     <col customWidth="1" min="2" max="6" width="14.43"/>
-    <col customWidth="1" min="9" max="9" width="10.0"/>
-    <col customWidth="1" min="10" max="10" width="9.71"/>
+    <col customWidth="1" min="8" max="8" width="10.0"/>
+    <col customWidth="1" min="9" max="9" width="9.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -477,7 +459,6 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
     </row>
     <row r="2" ht="30.75" customHeight="1">
       <c r="A2" s="1"/>
@@ -490,8 +471,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="4"/>
+      <c r="I2" s="4"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="5"/>
@@ -502,8 +482,7 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="7"/>
+      <c r="I3" s="7"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="8"/>
@@ -516,8 +495,7 @@
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="7"/>
+      <c r="I4" s="7"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="10"/>
@@ -531,9 +509,8 @@
       <c r="G5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="7"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="7"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="10"/>
@@ -547,9 +524,8 @@
       <c r="G6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="7"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="7"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="10"/>
@@ -563,9 +539,8 @@
       <c r="G7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="10"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="7"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="7"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="5"/>
@@ -575,9 +550,8 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="7"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="7"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="5"/>
@@ -588,8 +562,7 @@
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="7"/>
+      <c r="I9" s="7"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="13"/>
@@ -603,13 +576,12 @@
       <c r="G10" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="16"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="7"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="7"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="15"/>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="5"/>
@@ -619,124 +591,113 @@
       <c r="G11" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="10"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="7"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="7"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="15"/>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="22"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="21"/>
       <c r="G12" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="16"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="7"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="7"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="15"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="22"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="21"/>
       <c r="G13" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="16"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="7"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="7"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="15"/>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="7"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="7"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="22"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="7"/>
+      <c r="A15" s="21"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="7"/>
     </row>
     <row r="16" ht="30.0" customHeight="1">
-      <c r="A16" s="22"/>
-      <c r="B16" s="28" t="s">
+      <c r="A16" s="21"/>
+      <c r="B16" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="29" t="s">
+      <c r="D16" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="29" t="s">
+      <c r="E16" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="30" t="s">
+      <c r="F16" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="30" t="s">
+      <c r="G16" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="31" t="s">
+      <c r="H16" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="30" t="s">
+      <c r="I16" s="29" t="s">
         <v>22</v>
-      </c>
-      <c r="J16" s="32" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="10"/>
       <c r="B17" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="D17" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="E17" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="F17" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="G17" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="H17" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="H17" s="33" t="s">
+      <c r="I17" s="30" t="s">
         <v>30</v>
-      </c>
-      <c r="I17" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="J17" s="34" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
@@ -748,23 +709,21 @@
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="7"/>
+      <c r="I18" s="7"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="35"/>
-      <c r="B19" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="38" t="s">
-        <v>34</v>
+      <c r="A19" s="31"/>
+      <c r="B19" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="34" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1"/>
@@ -1751,7 +1710,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B12:D13"/>
-    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B2:I2"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>